<commit_message>
Excel control de trabajo con pesos
</commit_message>
<xml_diff>
--- a/_docs_/Ficha técnica/v2/reparto de tareas con pesos.xlsx
+++ b/_docs_/Ficha técnica/v2/reparto de tareas con pesos.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -127,7 +128,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,27 +166,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="0"/>
@@ -437,7 +417,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$I$2:$K$2</c:f>
+              <c:f>Hoja2!$A$2:$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -454,7 +434,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$24:$K$24</c:f>
+              <c:f>Hoja2!$A$24:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1389,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,10 +1383,9 @@
     <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="106.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="106.5" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1416,17 +1395,8 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1445,20 +1415,8 @@
       <c r="G3">
         <v>5</v>
       </c>
-      <c r="I3" s="3">
-        <f>C3*G3</f>
-        <v>50</v>
-      </c>
-      <c r="J3" s="3">
-        <f>D3*G3</f>
-        <v>100</v>
-      </c>
-      <c r="K3" s="3">
-        <f>E3*G3</f>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1471,20 +1429,8 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="I4" s="3">
-        <f t="shared" ref="I4:I22" si="0">C4*G4</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4:J22" si="1">D4*G4</f>
-        <v>200</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" ref="K4:K22" si="2">E4*G4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1494,20 +1440,8 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1523,20 +1457,8 @@
       <c r="G6">
         <v>20</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1552,20 +1474,8 @@
       <c r="G7">
         <v>5</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -1581,20 +1491,8 @@
       <c r="G8">
         <v>5</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1610,20 +1508,8 @@
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
-        <v>170</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="2"/>
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1639,20 +1525,8 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1668,20 +1542,8 @@
       <c r="G11">
         <v>10</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -1694,20 +1556,8 @@
       <c r="G12">
         <v>4</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="1"/>
-        <v>388</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1720,20 +1570,8 @@
       <c r="G13">
         <v>3</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="1"/>
-        <v>270</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -1743,20 +1581,8 @@
       <c r="G14">
         <v>10</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -1766,20 +1592,8 @@
       <c r="G15">
         <v>5</v>
       </c>
-      <c r="I15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <f t="shared" si="1"/>
-        <v>500</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -1789,20 +1603,8 @@
       <c r="G16">
         <v>2</v>
       </c>
-      <c r="I16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1812,20 +1614,8 @@
       <c r="G17">
         <v>2</v>
       </c>
-      <c r="I17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1835,20 +1625,8 @@
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="I18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -1858,20 +1636,8 @@
       <c r="G19">
         <v>4</v>
       </c>
-      <c r="I19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1887,20 +1653,8 @@
       <c r="G20">
         <v>6</v>
       </c>
-      <c r="I20" s="3">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1916,20 +1670,8 @@
       <c r="G21">
         <v>3</v>
       </c>
-      <c r="I21" s="3">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="J21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1939,45 +1681,16 @@
       <c r="G22">
         <v>3</v>
       </c>
-      <c r="I22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="3">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G24">
         <f>SUM(G3:G22)</f>
         <v>100</v>
       </c>
-      <c r="I24" s="3">
-        <f>SUM(I3:I22)</f>
-        <v>3980</v>
-      </c>
-      <c r="J24" s="3">
-        <f t="shared" ref="J24:K24" si="3">SUM(J3:J22)</f>
-        <v>4843</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="3"/>
-        <v>1177</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:E3">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C$3+$D$3+$E$3&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1985,4 +1698,328 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="5" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="106.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>Hoja1!C3*Hoja1!G3</f>
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <f>Hoja1!D3*Hoja1!G3</f>
+        <v>100</v>
+      </c>
+      <c r="C3" s="3">
+        <f>Hoja1!E3*Hoja1!G3</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f>Hoja1!C4*Hoja1!G4</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <f>Hoja1!D4*Hoja1!G4</f>
+        <v>200</v>
+      </c>
+      <c r="C4" s="3">
+        <f>Hoja1!E4*Hoja1!G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f>Hoja1!C5*Hoja1!G5</f>
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <f>Hoja1!D5*Hoja1!G5</f>
+        <v>200</v>
+      </c>
+      <c r="C5" s="3">
+        <f>Hoja1!E5*Hoja1!G5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f>Hoja1!C6*Hoja1!G6</f>
+        <v>1800</v>
+      </c>
+      <c r="B6" s="3">
+        <f>Hoja1!D6*Hoja1!G6</f>
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <f>Hoja1!E6*Hoja1!G6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f>Hoja1!C7*Hoja1!G7</f>
+        <v>450</v>
+      </c>
+      <c r="B7" s="3">
+        <f>Hoja1!D7*Hoja1!G7</f>
+        <v>40</v>
+      </c>
+      <c r="C7" s="3">
+        <f>Hoja1!E7*Hoja1!G7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f>Hoja1!C8*Hoja1!G8</f>
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <f>Hoja1!D8*Hoja1!G8</f>
+        <v>400</v>
+      </c>
+      <c r="C8" s="3">
+        <f>Hoja1!E8*Hoja1!G8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f>Hoja1!C9*Hoja1!G9</f>
+        <v>170</v>
+      </c>
+      <c r="B9" s="3">
+        <f>Hoja1!D9*Hoja1!G9</f>
+        <v>165</v>
+      </c>
+      <c r="C9" s="3">
+        <f>Hoja1!E9*Hoja1!G9</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f>Hoja1!C10*Hoja1!G10</f>
+        <v>110</v>
+      </c>
+      <c r="B10" s="3">
+        <f>Hoja1!D10*Hoja1!G10</f>
+        <v>90</v>
+      </c>
+      <c r="C10" s="3">
+        <f>Hoja1!E10*Hoja1!G10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f>Hoja1!C11*Hoja1!G11</f>
+        <v>900</v>
+      </c>
+      <c r="B11" s="3">
+        <f>Hoja1!D11*Hoja1!G11</f>
+        <v>90</v>
+      </c>
+      <c r="C11" s="3">
+        <f>Hoja1!E11*Hoja1!G11</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f>Hoja1!C12*Hoja1!G12</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
+        <f>Hoja1!D12*Hoja1!G12</f>
+        <v>388</v>
+      </c>
+      <c r="C12" s="3">
+        <f>Hoja1!E12*Hoja1!G12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f>Hoja1!C13*Hoja1!G13</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <f>Hoja1!D13*Hoja1!G13</f>
+        <v>270</v>
+      </c>
+      <c r="C13" s="3">
+        <f>Hoja1!E13*Hoja1!G13</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>Hoja1!C14*Hoja1!G14</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="3">
+        <f>Hoja1!D14*Hoja1!G14</f>
+        <v>1000</v>
+      </c>
+      <c r="C14" s="3">
+        <f>Hoja1!E14*Hoja1!G14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f>Hoja1!C15*Hoja1!G15</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="3">
+        <f>Hoja1!D15*Hoja1!G15</f>
+        <v>500</v>
+      </c>
+      <c r="C15" s="3">
+        <f>Hoja1!E15*Hoja1!G15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f>Hoja1!C16*Hoja1!G16</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
+        <f>Hoja1!D16*Hoja1!G16</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <f>Hoja1!E16*Hoja1!G16</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f>Hoja1!C17*Hoja1!G17</f>
+        <v>0</v>
+      </c>
+      <c r="B17" s="3">
+        <f>Hoja1!D17*Hoja1!G17</f>
+        <v>200</v>
+      </c>
+      <c r="C17" s="3">
+        <f>Hoja1!E17*Hoja1!G17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f>Hoja1!C18*Hoja1!G18</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="3">
+        <f>Hoja1!D18*Hoja1!G18</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <f>Hoja1!E18*Hoja1!G18</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f>Hoja1!C19*Hoja1!G19</f>
+        <v>0</v>
+      </c>
+      <c r="B19" s="3">
+        <f>Hoja1!D19*Hoja1!G19</f>
+        <v>400</v>
+      </c>
+      <c r="C19" s="3">
+        <f>Hoja1!E19*Hoja1!G19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f>Hoja1!C20*Hoja1!G20</f>
+        <v>300</v>
+      </c>
+      <c r="B20" s="3">
+        <f>Hoja1!D20*Hoja1!G20</f>
+        <v>300</v>
+      </c>
+      <c r="C20" s="3">
+        <f>Hoja1!E20*Hoja1!G20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f>Hoja1!C21*Hoja1!G21</f>
+        <v>150</v>
+      </c>
+      <c r="B21" s="3">
+        <f>Hoja1!D21*Hoja1!G21</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <f>Hoja1!E21*Hoja1!G21</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f>Hoja1!C22*Hoja1!G22</f>
+        <v>0</v>
+      </c>
+      <c r="B22" s="3">
+        <f>Hoja1!D22*Hoja1!G22</f>
+        <v>300</v>
+      </c>
+      <c r="C22" s="3">
+        <f>Hoja1!E22*Hoja1!G22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>SUM(A3:A22)</f>
+        <v>3980</v>
+      </c>
+      <c r="B24" s="3">
+        <f>SUM(B3:B22)</f>
+        <v>4843</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C3:C22)</f>
+        <v>1177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel control de trabajo con pesos revisado
</commit_message>
<xml_diff>
--- a/_docs_/Ficha técnica/v2/reparto de tareas con pesos.xlsx
+++ b/_docs_/Ficha técnica/v2/reparto de tareas con pesos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Cristina Perea</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Vistas</t>
   </si>
   <si>
-    <t>Modelos</t>
-  </si>
-  <si>
     <t>Utilidades</t>
   </si>
   <si>
@@ -112,6 +109,12 @@
   </si>
   <si>
     <t>Elaboración de la presentación PowerPoint</t>
+  </si>
+  <si>
+    <t>PESO</t>
+  </si>
+  <si>
+    <t>Modelos de clases</t>
   </si>
 </sst>
 </file>
@@ -133,15 +136,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,11 +164,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -162,11 +192,23 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -439,13 +481,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3980</c:v>
+                  <c:v>4425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4843</c:v>
+                  <c:v>4716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1177</c:v>
+                  <c:v>849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,13 +1118,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>581026</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>207066</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
@@ -1371,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,9 +1422,9 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="106.5" x14ac:dyDescent="0.25">
@@ -1395,6 +1437,9 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1403,16 +1448,16 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>70</v>
-      </c>
-      <c r="G3">
+      <c r="C3" s="4">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5">
         <v>5</v>
       </c>
     </row>
@@ -1423,22 +1468,26 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="G4">
-        <v>2</v>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
         <v>100</v>
       </c>
-      <c r="G5">
-        <v>2</v>
+      <c r="E5" s="4"/>
+      <c r="G5" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,13 +1497,14 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>90</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="E6" s="4"/>
+      <c r="G6" s="5">
         <v>20</v>
       </c>
     </row>
@@ -1462,33 +1512,33 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>90</v>
       </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="G7">
+      <c r="D7" s="4">
         <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>80</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="G8">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>90</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
         <v>5</v>
       </c>
     </row>
@@ -1496,16 +1546,16 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>34</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="4">
         <v>33</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="4">
         <v>33</v>
       </c>
-      <c r="G9">
+      <c r="E9" s="4">
+        <v>33</v>
+      </c>
+      <c r="G9" s="5">
         <v>5</v>
       </c>
     </row>
@@ -1516,125 +1566,140 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
-        <v>55</v>
-      </c>
-      <c r="D10">
-        <v>45</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
+      <c r="C10" s="4">
+        <v>60</v>
+      </c>
+      <c r="D10" s="4">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="G10" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>90</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
         <v>97</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>4</v>
+      <c r="G12" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4">
         <v>90</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>10</v>
       </c>
-      <c r="G13">
-        <v>3</v>
+      <c r="G13" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
         <v>100</v>
       </c>
-      <c r="G14">
+      <c r="E14" s="4"/>
+      <c r="G14" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4">
         <v>100</v>
       </c>
-      <c r="G15">
-        <v>5</v>
+      <c r="E15" s="4"/>
+      <c r="G15" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
         <v>100</v>
       </c>
-      <c r="G16">
-        <v>2</v>
+      <c r="G16" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4">
         <v>100</v>
       </c>
-      <c r="G17">
-        <v>2</v>
+      <c r="E17" s="4"/>
+      <c r="G17" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
         <v>100</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4">
         <v>100</v>
       </c>
-      <c r="G19">
-        <v>4</v>
+      <c r="E19" s="4"/>
+      <c r="G19" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,16 +1707,17 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4">
         <v>50</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>50</v>
       </c>
-      <c r="G20">
-        <v>6</v>
+      <c r="E20" s="4"/>
+      <c r="G20" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1659,15 +1725,16 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <v>50</v>
-      </c>
-      <c r="G21">
+        <v>27</v>
+      </c>
+      <c r="C21" s="4">
+        <v>60</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4">
+        <v>40</v>
+      </c>
+      <c r="G21" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1675,10 +1742,12 @@
       <c r="B22" t="s">
         <v>17</v>
       </c>
-      <c r="D22">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4">
         <v>100</v>
       </c>
-      <c r="G22">
+      <c r="E22" s="4"/>
+      <c r="G22" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1689,11 +1758,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:E3">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$C$3+$D$3+$E$3&lt;&gt;100</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1705,7 +1769,7 @@
   <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,15 +1791,15 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>Hoja1!C3*Hoja1!G3</f>
-        <v>50</v>
+        <v>165</v>
       </c>
       <c r="B3" s="3">
         <f>Hoja1!D3*Hoja1!G3</f>
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3">
         <f>Hoja1!E3*Hoja1!G3</f>
-        <v>350</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1745,7 +1809,7 @@
       </c>
       <c r="B4" s="3">
         <f>Hoja1!D4*Hoja1!G4</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3">
         <f>Hoja1!E4*Hoja1!G4</f>
@@ -1759,7 +1823,7 @@
       </c>
       <c r="B5" s="3">
         <f>Hoja1!D5*Hoja1!G5</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3">
         <f>Hoja1!E5*Hoja1!G5</f>
@@ -1783,35 +1847,35 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f>Hoja1!C7*Hoja1!G7</f>
-        <v>450</v>
+        <v>630</v>
       </c>
       <c r="B7" s="3">
         <f>Hoja1!D7*Hoja1!G7</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3">
         <f>Hoja1!E7*Hoja1!G7</f>
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f>Hoja1!C8*Hoja1!G8</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <f>Hoja1!D8*Hoja1!G8</f>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="C8" s="3">
         <f>Hoja1!E8*Hoja1!G8</f>
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f>Hoja1!C9*Hoja1!G9</f>
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B9" s="3">
         <f>Hoja1!D9*Hoja1!G9</f>
@@ -1825,11 +1889,11 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f>Hoja1!C10*Hoja1!G10</f>
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3">
         <f>Hoja1!D10*Hoja1!G10</f>
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3">
         <f>Hoja1!E10*Hoja1!G10</f>
@@ -1857,11 +1921,11 @@
       </c>
       <c r="B12" s="3">
         <f>Hoja1!D12*Hoja1!G12</f>
-        <v>388</v>
+        <v>291</v>
       </c>
       <c r="C12" s="3">
         <f>Hoja1!E12*Hoja1!G12</f>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,11 +1935,11 @@
       </c>
       <c r="B13" s="3">
         <f>Hoja1!D13*Hoja1!G13</f>
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="C13" s="3">
         <f>Hoja1!E13*Hoja1!G13</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,7 +1963,7 @@
       </c>
       <c r="B15" s="3">
         <f>Hoja1!D15*Hoja1!G15</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="C15" s="3">
         <f>Hoja1!E15*Hoja1!G15</f>
@@ -1917,7 +1981,7 @@
       </c>
       <c r="C16" s="3">
         <f>Hoja1!E16*Hoja1!G16</f>
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1991,7 @@
       </c>
       <c r="B17" s="3">
         <f>Hoja1!D17*Hoja1!G17</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C17" s="3">
         <f>Hoja1!E17*Hoja1!G17</f>
@@ -1955,7 +2019,7 @@
       </c>
       <c r="B19" s="3">
         <f>Hoja1!D19*Hoja1!G19</f>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="C19" s="3">
         <f>Hoja1!E19*Hoja1!G19</f>
@@ -1965,11 +2029,11 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f>Hoja1!C20*Hoja1!G20</f>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="B20" s="3">
         <f>Hoja1!D20*Hoja1!G20</f>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C20" s="3">
         <f>Hoja1!E20*Hoja1!G20</f>
@@ -1979,7 +2043,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f>Hoja1!C21*Hoja1!G21</f>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B21" s="3">
         <f>Hoja1!D21*Hoja1!G21</f>
@@ -1987,7 +2051,7 @@
       </c>
       <c r="C21" s="3">
         <f>Hoja1!E21*Hoja1!G21</f>
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2007,15 +2071,15 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f>SUM(A3:A22)</f>
-        <v>3980</v>
+        <v>4425</v>
       </c>
       <c r="B24" s="3">
         <f>SUM(B3:B22)</f>
-        <v>4843</v>
+        <v>4716</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C3:C22)</f>
-        <v>1177</v>
+        <v>849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>